<commit_message>
Reteste da parametrização - marcado com " 21-09-13- 12 h 22 m"
</commit_message>
<xml_diff>
--- a/Apresentacao 3/slide_oprime_fracos.xlsx
+++ b/Apresentacao 3/slide_oprime_fracos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fj428\Documents\GitHub\metaheuristicas\Apresentacao 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ED55D68-396F-4198-8FE8-68D0EEB66556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D82F20-B724-4FA5-9244-825F521A09F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B242CD8-D37E-4745-A0C1-18E0456D1F4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="18">
   <si>
     <t>Objetivos</t>
   </si>
@@ -64,19 +65,55 @@
   </si>
   <si>
     <t>inicial</t>
+  </si>
+  <si>
+    <t>Indivíduo gerado</t>
+  </si>
+  <si>
+    <t>Cruzamento simples</t>
+  </si>
+  <si>
+    <t>Cruzamento aleatório</t>
+  </si>
+  <si>
+    <t>Sorteio</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Parente A</t>
+  </si>
+  <si>
+    <t>Parente B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="LM Roman 10"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -117,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -125,6 +162,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,7 +889,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,4 +1009,479 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5757B06D-A876-4C7A-AC2A-EAE8A5BF5A84}">
+  <dimension ref="A2:AA11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="2.44140625" customWidth="1"/>
+    <col min="4" max="13" width="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" customWidth="1"/>
+    <col min="16" max="16" width="2.44140625" customWidth="1"/>
+    <col min="17" max="26" width="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="6"/>
+    </row>
+    <row r="4" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" s="6"/>
+    </row>
+    <row r="6" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="8">
+        <v>1</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0</v>
+      </c>
+      <c r="S7" s="8">
+        <v>0</v>
+      </c>
+      <c r="T7" s="9">
+        <v>1</v>
+      </c>
+      <c r="U7" s="9">
+        <v>1</v>
+      </c>
+      <c r="V7" s="9">
+        <v>1</v>
+      </c>
+      <c r="W7" s="9">
+        <v>0</v>
+      </c>
+      <c r="X7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" ht="18" x14ac:dyDescent="0.45">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" ht="36" x14ac:dyDescent="0.45">
+      <c r="A10" s="5"/>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="W10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="X10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="O3:Z3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>